<commit_message>
Added all .gro staring structures
</commit_message>
<xml_diff>
--- a/Fluoride assay/Fluoride Interference assay/Fluoride Assay Interference Table.xlsx
+++ b/Fluoride assay/Fluoride Interference assay/Fluoride Assay Interference Table.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eawag\userdata\felderfl\My Documents\GitHub\fluorinated_compounds_biotransformations\data\Fluoride Interference assay\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eawag\userdata\felderfl\My Documents\GitHub\biodefluorination-paper\Fluoride assay\Fluoride Interference assay\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="48">
   <si>
     <t>Component</t>
   </si>
@@ -162,6 +163,12 @@
   </si>
   <si>
     <t>10 mM Tricine</t>
+  </si>
+  <si>
+    <t>Not interfering</t>
+  </si>
+  <si>
+    <t>Interfering</t>
   </si>
 </sst>
 </file>
@@ -204,7 +211,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -278,11 +285,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFD9D9D9"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFD9D9D9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -301,6 +319,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -582,323 +612,438 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B45"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="49.54296875" customWidth="1"/>
     <col min="2" max="2" width="65.7265625" customWidth="1"/>
+    <col min="6" max="6" width="36.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F4" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>0</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>0</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F6" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>0</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>0</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F8" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>0</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>0</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>0</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F11" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>0</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F12" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>0</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F13" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>0</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F14" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>0</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F15" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>0</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F16" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>0</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F17" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>0</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F18" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>0</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F19" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>0</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F20" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>0</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>0</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F22" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>0</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F23" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>0</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F24" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>0</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F25" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>0</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F26" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>0</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F27" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>0</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F28" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>0</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F29" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>0</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F30" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>0</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F31" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>0</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F32" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <v>1</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F33" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <v>1</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F34" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="70.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>1</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F35" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F36" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="84.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <v>0</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F37" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="84.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3">
         <v>0</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="F38" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3">
         <v>0</v>
       </c>
@@ -906,56 +1051,283 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="6">
         <v>0</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F40" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="6">
         <v>1</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F41" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="6">
         <v>1</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F42" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="42.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="6">
         <v>1</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F43" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="56.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="6">
         <v>0</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="F44" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="84" x14ac:dyDescent="0.35">
       <c r="A45" s="6">
         <v>0</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>34</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="84" x14ac:dyDescent="0.35">
+      <c r="F46" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="84" x14ac:dyDescent="0.35">
+      <c r="F47" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="A1:C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" customWidth="1"/>
+    <col min="3" max="3" width="20.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="35" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>